<commit_message>
pep8 + better datestamp finally
</commit_message>
<xml_diff>
--- a/data_exploration.xlsx
+++ b/data_exploration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-920" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Image Classes" sheetId="1" r:id="rId1"/>
@@ -966,7 +966,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -974,11 +973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1324351952"/>
-        <c:axId val="-2075734960"/>
+        <c:axId val="-2018174432"/>
+        <c:axId val="-2075251776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1324351952"/>
+        <c:axId val="-2018174432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,12 +1081,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2075734960"/>
+        <c:crossAx val="-2075251776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2075734960"/>
+        <c:axId val="-2075251776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200000.0"/>
@@ -1201,7 +1200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1324351952"/>
+        <c:crossAx val="-2018174432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1764,6 +1763,21 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Lesioning!$A$3:$A$22</c:f>
@@ -1946,6 +1960,21 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Lesioning!$A$3:$A$22</c:f>
@@ -2094,11 +2123,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1299440688"/>
-        <c:axId val="-2042371760"/>
+        <c:axId val="1051810432"/>
+        <c:axId val="1052253152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1299440688"/>
+        <c:axId val="1051810432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2202,12 +2231,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042371760"/>
+        <c:crossAx val="1052253152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2042371760"/>
+        <c:axId val="1052253152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.25"/>
@@ -2321,7 +2350,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1299440688"/>
+        <c:crossAx val="1051810432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3549,13 +3578,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>393700</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>393700</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -5199,8 +5228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>